<commit_message>
Correct LA metiers with extra zero
</commit_message>
<xml_diff>
--- a/Metiers/Reference_lists/RDB_ISSG_Metier_list.xlsx
+++ b/Metiers/Reference_lists/RDB_ISSG_Metier_list.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Metier list final'!$A$1:$L$1639</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7470,9 +7470,6 @@
     <t>LA_SLP_&gt;0_0_0</t>
   </si>
   <si>
-    <t>LA_SLP_&lt;14_0_0_0</t>
-  </si>
-  <si>
     <t>Lamprette, Small and large pelagic species, see the coe reg. mesh size ans selectivity device</t>
   </si>
   <si>
@@ -7530,15 +7527,9 @@
     <t>LA_LPF_&gt;0_0_0</t>
   </si>
   <si>
-    <t>LA_LPF_&lt;14_0_0_0</t>
-  </si>
-  <si>
     <t>LA_LPF_&gt;=14_0_0</t>
   </si>
   <si>
-    <t>LA_SPF_&lt;14_0_0_0</t>
-  </si>
-  <si>
     <t>LA_SPF_&gt;=14_0_0</t>
   </si>
   <si>
@@ -7576,6 +7567,15 @@
   </si>
   <si>
     <t>Request from Spain</t>
+  </si>
+  <si>
+    <t>LA_LPF_&lt;14_0_0</t>
+  </si>
+  <si>
+    <t>LA_SLP_&lt;14_0_0</t>
+  </si>
+  <si>
+    <t>LA_SPF_&lt;14_0_0</t>
   </si>
 </sst>
 </file>
@@ -8392,7 +8392,7 @@
   <dimension ref="A1:AD1639"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8447,7 +8447,7 @@
         <v>1974</v>
       </c>
       <c r="L1" s="88" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -13241,7 +13241,7 @@
         <v>1276</v>
       </c>
       <c r="B231" s="78" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="H231" s="86" t="s">
         <v>1710</v>
@@ -13311,7 +13311,7 @@
         <v>1276</v>
       </c>
       <c r="B236" s="78" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="H236" s="86" t="s">
         <v>1626</v>
@@ -13381,7 +13381,7 @@
         <v>1276</v>
       </c>
       <c r="B241" s="78" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="H241" s="86" t="s">
         <v>1629</v>
@@ -13465,7 +13465,7 @@
         <v>1276</v>
       </c>
       <c r="B247" s="78" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="H247" s="86" t="s">
         <v>1633</v>
@@ -13880,7 +13880,7 @@
         <v>20221214</v>
       </c>
       <c r="L272" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.3">
@@ -13888,7 +13888,7 @@
         <v>1276</v>
       </c>
       <c r="B273" s="8" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="C273" s="8"/>
       <c r="D273" s="8"/>
@@ -13905,7 +13905,7 @@
         <v>20221214</v>
       </c>
       <c r="L273" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.3">
@@ -13930,7 +13930,7 @@
         <v>20221214</v>
       </c>
       <c r="L274" s="8" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.3">
@@ -13988,14 +13988,14 @@
         <v>1608</v>
       </c>
       <c r="I278" s="8" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="J278" s="8"/>
       <c r="K278" s="8">
         <v>20221214</v>
       </c>
       <c r="L278" s="8" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
@@ -14011,14 +14011,14 @@
         <v>1608</v>
       </c>
       <c r="I279" s="8" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="J279" s="8"/>
       <c r="K279" s="8">
         <v>20221214</v>
       </c>
       <c r="L279" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.3">
@@ -14026,7 +14026,7 @@
         <v>1276</v>
       </c>
       <c r="B280" s="8" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="C280" s="8"/>
       <c r="D280" s="8"/>
@@ -14034,14 +14034,14 @@
         <v>1608</v>
       </c>
       <c r="I280" s="8" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="J280" s="8"/>
       <c r="K280" s="8">
         <v>20221214</v>
       </c>
       <c r="L280" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
@@ -14138,7 +14138,7 @@
         <v>1276</v>
       </c>
       <c r="B287" s="28" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="C287" s="15"/>
       <c r="D287" s="3"/>
@@ -14313,7 +14313,7 @@
         <v>1276</v>
       </c>
       <c r="B297" s="25" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="H297" s="86" t="s">
         <v>1704</v>
@@ -14585,7 +14585,7 @@
         <v>1277</v>
       </c>
       <c r="B316" s="91" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="C316" s="8"/>
       <c r="D316" s="8"/>
@@ -14600,7 +14600,7 @@
         <v>20221214</v>
       </c>
       <c r="L316" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.3">
@@ -14608,7 +14608,7 @@
         <v>1277</v>
       </c>
       <c r="B317" s="91" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="C317" s="8"/>
       <c r="D317" s="8"/>
@@ -14623,7 +14623,7 @@
         <v>20221214</v>
       </c>
       <c r="L317" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.3">
@@ -14646,7 +14646,7 @@
         <v>20221214</v>
       </c>
       <c r="L318" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.3">
@@ -14948,7 +14948,7 @@
         <v>1277</v>
       </c>
       <c r="B340" s="91" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="C340" s="8"/>
       <c r="D340" s="8"/>
@@ -14961,7 +14961,7 @@
         <v>20221214</v>
       </c>
       <c r="L340" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.3">
@@ -14969,7 +14969,7 @@
         <v>1277</v>
       </c>
       <c r="B341" s="91" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="C341" s="8"/>
       <c r="D341" s="8"/>
@@ -14982,7 +14982,7 @@
         <v>20221214</v>
       </c>
       <c r="L341" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.3">
@@ -15003,7 +15003,7 @@
         <v>20221214</v>
       </c>
       <c r="L342" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="343" spans="1:12" x14ac:dyDescent="0.3">
@@ -15179,22 +15179,22 @@
         <v>1277</v>
       </c>
       <c r="B355" s="91" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="C355" s="8"/>
       <c r="D355" s="8"/>
       <c r="H355" s="90" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="I355" s="8" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="J355" s="8"/>
       <c r="K355" s="8">
         <v>20221214</v>
       </c>
       <c r="L355" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.3">
@@ -15202,22 +15202,22 @@
         <v>1277</v>
       </c>
       <c r="B356" s="91" t="s">
-        <v>2077</v>
+        <v>2090</v>
       </c>
       <c r="C356" s="8"/>
       <c r="D356" s="8"/>
       <c r="H356" s="90" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="I356" s="8" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="J356" s="8"/>
       <c r="K356" s="8">
         <v>20221214</v>
       </c>
       <c r="L356" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.3">
@@ -15225,22 +15225,22 @@
         <v>1277</v>
       </c>
       <c r="B357" s="91" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="C357" s="8"/>
       <c r="D357" s="8"/>
       <c r="H357" s="90" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="I357" s="8" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="J357" s="8"/>
       <c r="K357" s="8">
         <v>20221214</v>
       </c>
       <c r="L357" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.3">
@@ -15256,14 +15256,14 @@
         <v>2055</v>
       </c>
       <c r="I358" s="8" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="J358" s="8"/>
       <c r="K358" s="8">
         <v>20221214</v>
       </c>
       <c r="L358" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.3">
@@ -15271,7 +15271,7 @@
         <v>1277</v>
       </c>
       <c r="B359" s="91" t="s">
-        <v>2057</v>
+        <v>2091</v>
       </c>
       <c r="C359" s="8"/>
       <c r="D359" s="8"/>
@@ -15279,14 +15279,14 @@
         <v>2055</v>
       </c>
       <c r="I359" s="8" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="J359" s="8"/>
       <c r="K359" s="8">
         <v>20221214</v>
       </c>
       <c r="L359" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.3">
@@ -15302,14 +15302,14 @@
         <v>2055</v>
       </c>
       <c r="I360" s="8" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="J360" s="8"/>
       <c r="K360" s="8">
         <v>20221214</v>
       </c>
       <c r="L360" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.3">
@@ -15325,14 +15325,14 @@
         <v>1730</v>
       </c>
       <c r="I361" s="8" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="J361" s="8"/>
       <c r="K361" s="8">
         <v>20221214</v>
       </c>
       <c r="L361" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.3">
@@ -15340,7 +15340,7 @@
         <v>1277</v>
       </c>
       <c r="B362" s="91" t="s">
-        <v>2079</v>
+        <v>2092</v>
       </c>
       <c r="C362" s="8"/>
       <c r="D362" s="8"/>
@@ -15348,14 +15348,14 @@
         <v>1730</v>
       </c>
       <c r="I362" s="8" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="J362" s="8"/>
       <c r="K362" s="8">
         <v>20221214</v>
       </c>
       <c r="L362" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.3">
@@ -15363,7 +15363,7 @@
         <v>1277</v>
       </c>
       <c r="B363" s="91" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="C363" s="8"/>
       <c r="D363" s="8"/>
@@ -15371,14 +15371,14 @@
         <v>1730</v>
       </c>
       <c r="I363" s="8" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="J363" s="8"/>
       <c r="K363" s="8">
         <v>20221214</v>
       </c>
       <c r="L363" s="8" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.3">
@@ -15457,7 +15457,7 @@
         <v>20221214</v>
       </c>
       <c r="L368" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.3">
@@ -15536,7 +15536,7 @@
         <v>20221214</v>
       </c>
       <c r="L373" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.3">
@@ -15615,7 +15615,7 @@
         <v>20221214</v>
       </c>
       <c r="L378" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.3">
@@ -15631,14 +15631,14 @@
         <v>1587</v>
       </c>
       <c r="I379" s="8" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="J379" s="8"/>
       <c r="K379" s="8">
         <v>20221214</v>
       </c>
       <c r="L379" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.3">
@@ -15738,14 +15738,14 @@
         <v>1678</v>
       </c>
       <c r="I386" s="8" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="J386" s="8"/>
       <c r="K386" s="8">
         <v>20221214</v>
       </c>
       <c r="L386" s="8" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.3">
@@ -15753,22 +15753,22 @@
         <v>1277</v>
       </c>
       <c r="B387" s="91" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="C387" s="8"/>
       <c r="D387" s="8"/>
       <c r="H387" s="90" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="I387" s="8" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="J387" s="8"/>
       <c r="K387" s="8">
         <v>20221214</v>
       </c>
       <c r="L387" s="8" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.3">
@@ -16699,22 +16699,22 @@
         <v>1277</v>
       </c>
       <c r="B449" s="91" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="C449" s="8"/>
       <c r="D449" s="8"/>
       <c r="H449" s="90" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="I449" s="8" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="J449" s="8"/>
       <c r="K449" s="8">
         <v>20221214</v>
       </c>
       <c r="L449" s="8" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>